<commit_message>
change algorithm  of database change in get_cost and get_product
</commit_message>
<xml_diff>
--- a/database/industries/folad/fakhouz/cost/yearly/cost.xlsx
+++ b/database/industries/folad/fakhouz/cost/yearly/cost.xlsx
@@ -1,15 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Trade\database\industries\folad\fakhouz\cost\yearly\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -195,8 +200,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -259,6 +264,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -305,7 +318,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -337,9 +350,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -371,6 +385,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -546,14 +561,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="28.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="6" width="20.5703125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1">
         <v>0</v>
       </c>
@@ -573,7 +594,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>14</v>
       </c>
@@ -590,7 +611,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -610,7 +631,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -630,7 +651,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -650,7 +671,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>3</v>
       </c>
@@ -670,7 +691,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -690,7 +711,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>5</v>
       </c>
@@ -710,7 +731,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>6</v>
       </c>
@@ -730,7 +751,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>7</v>
       </c>
@@ -750,7 +771,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>8</v>
       </c>
@@ -770,7 +791,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>9</v>
       </c>
@@ -790,7 +811,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>10</v>
       </c>
@@ -810,7 +831,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>11</v>
       </c>
@@ -830,7 +851,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>12</v>
       </c>
@@ -850,7 +871,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>13</v>
       </c>

</xml_diff>